<commit_message>
add cooldown module drop item module
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel/IObject.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,17 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
+    <sheet name="Record_Cooldown" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Record_Cooldown!$A$1:$B$11</definedName>
+  </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
@@ -79,12 +83,27 @@
   </si>
   <si>
     <t>Upload</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Col</t>
+  </si>
+  <si>
+    <t>Cooldown</t>
+  </si>
+  <si>
+    <t>SkillID</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -107,7 +126,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +145,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -257,7 +282,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -298,6 +323,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -645,10 +688,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
@@ -881,8 +924,8 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 B7:H9 F10:F1048576 F2:F6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 B7:H9 F10:F1048576 F2:F6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -890,4 +933,120 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E278CF-F7E2-4D32-8235-E83F81F9FE21}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="13.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="16" customFormat="1">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="17" customFormat="1">
+      <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="17" customFormat="1">
+      <c r="A3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="17" customFormat="1">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="17" customFormat="1">
+      <c r="A5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="17" customFormat="1">
+      <c r="A6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="17" customFormat="1">
+      <c r="A7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="17" customFormat="1">
+      <c r="A8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="17" customFormat="1">
+      <c r="A9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="17" customFormat="1">
+      <c r="A10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="17" customFormat="1">
+      <c r="A11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="19"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:B3" xr:uid="{099D9AAA-F796-4EE8-B36B-E82AC4D6C782}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 C11:H11 C1:H8" xr:uid="{31B2A9F8-3FCB-4D3F-BF25-F136BB5A1DE2}">
+      <formula1>"int,string,float,object"</formula1>
+    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9" xr:uid="{A155630B-C656-415A-89F7-0C9BE6D22C3A}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B6 B7:B8" xr:uid="{F82A1EFB-D319-4BEA-92BB-D4D2299EBC91}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add guild properties fixed bugs for changing hero
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel/IObject.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -688,9 +688,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -765,8 +765,8 @@
       <c r="F3" s="10">
         <v>0</v>
       </c>
-      <c r="G3" s="10">
-        <v>1</v>
+      <c r="G3" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1">
@@ -819,23 +819,23 @@
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9">
-        <v>0</v>
+      <c r="B6" s="10">
+        <v>1</v>
       </c>
       <c r="C6" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="10">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1">
@@ -922,7 +922,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6 B7:H9 F10:F1048576 F2:F6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6 B7:H9 F10:F1048576 B6:E6 G3:G6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -936,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E278CF-F7E2-4D32-8235-E83F81F9FE21}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
dont save the ClassName and ConfigName
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel/IObject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="9930"/>
+    <workbookView windowWidth="17100" windowHeight="9930"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -108,12 +108,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -122,73 +129,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,26 +157,63 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -234,23 +225,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,13 +277,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,169 +397,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,6 +583,24 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,11 +635,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -643,30 +676,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -675,162 +684,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1272,7 +1272,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1402,10 +1402,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -1413,11 +1413,11 @@
       <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10">
-        <v>1</v>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:7">
@@ -1502,7 +1502,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:C6 F2:F6 F10:F1048576 G3:G6 B7:H9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5 F6 G6 F2:F5 F10:F1048576 G3:G4 B7:H9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
removed unused files modified the workflow for attaching the player data
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/IObject.xlsx
+++ b/_Out/NFDataCfg/Excel/IObject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21120"/>
+    <workbookView windowHeight="23360"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -84,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -119,6 +119,43 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -133,127 +170,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -261,6 +177,90 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -283,25 +283,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,19 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,7 +445,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,121 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,6 +608,63 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -633,210 +690,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1278,7 +1278,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1350,11 +1350,11 @@
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8">
-        <v>0</v>
+      <c r="B3" s="9">
+        <v>1</v>
       </c>
       <c r="C3" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="9">
         <v>0</v>
@@ -1363,16 +1363,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
       </c>
       <c r="H3" s="3">
         <v>0</v>
       </c>
       <c r="I3" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:9">
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -1563,7 +1563,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 I1 A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H4 H5 F6:G6 H6 I6 F2:F5 F10:F1048576 G3:G5 H7:H9 I2:I5 I7:I9 I10:I1048576 B7:G9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 I2 B3 C3 F3 G3 H3 I3 H4 H5 F6 G6 H6 I6 F4:F5 F10:F1048576 G4:G5 H7:H9 I4:I5 I7:I9 I10:I1048576 B7:G9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>